<commit_message>
Sprint 2 backlog updated
</commit_message>
<xml_diff>
--- a/Documentation/Sprint 2 Backlog.xlsx
+++ b/Documentation/Sprint 2 Backlog.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="36" windowWidth="11460" windowHeight="7956"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,12 @@
   <definedNames>
     <definedName name="Status">Sheet1!$K$1:$K$3</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -135,8 +140,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -225,11 +230,11 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -238,7 +243,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -246,17 +251,17 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -266,7 +271,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -274,57 +279,57 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -333,18 +338,18 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -417,6 +422,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,18 +441,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -739,40 +744,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="51.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" style="1" customWidth="1"/>
-    <col min="5" max="11" width="8.88671875" style="1"/>
-    <col min="12" max="13" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
+    <col min="5" max="11" width="8.83203125" style="1"/>
+    <col min="12" max="13" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="21">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:13" ht="20">
+      <c r="A1" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="23"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="27"/>
       <c r="J1"/>
       <c r="K1" s="8"/>
     </row>
@@ -968,7 +973,7 @@
       <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="21" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="3">
@@ -998,7 +1003,7 @@
       <c r="C12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="21" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="3">
@@ -1028,23 +1033,23 @@
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="24" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="3">
         <v>2</v>
       </c>
       <c r="F13" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I13" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13"/>
     </row>
@@ -1058,7 +1063,7 @@
       <c r="C14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="3">
@@ -1088,7 +1093,7 @@
       <c r="C15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="22" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="3">
@@ -1118,7 +1123,7 @@
       <c r="C16" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="23" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="19">
@@ -1172,19 +1177,19 @@
       </c>
       <c r="F19" s="3">
         <f t="shared" ref="F19:I19" si="0">SUM(F6:F16)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H19" s="3">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I19" s="3">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J19"/>
     </row>
@@ -1249,22 +1254,26 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="73" orientation="landscape" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1316,17 +1325,27 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>